<commit_message>
working on the comparison of SVs, Dumper print equal objects as a reference
</commit_message>
<xml_diff>
--- a/misc/SV-features.xlsx
+++ b/misc/SV-features.xlsx
@@ -11,8 +11,9 @@
     <sheet name="MANTA" sheetId="2" r:id="rId2"/>
     <sheet name="SVABA" sheetId="3" r:id="rId3"/>
     <sheet name="PON-SVAVA-MATCH" sheetId="4" r:id="rId4"/>
+    <sheet name="unique  per tool" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="270">
   <si>
     <t>CIEND</t>
   </si>
@@ -811,12 +812,36 @@
   </si>
   <si>
     <t>%PON</t>
+  </si>
+  <si>
+    <t>DEL</t>
+  </si>
+  <si>
+    <t>DUP</t>
+  </si>
+  <si>
+    <t>INS</t>
+  </si>
+  <si>
+    <t>INV</t>
+  </si>
+  <si>
+    <t>TRA</t>
+  </si>
+  <si>
+    <t>Delly</t>
+  </si>
+  <si>
+    <t>PONF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.0000"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -866,7 +891,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="55">
+  <cellStyleXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -922,8 +947,32 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -937,8 +986,14 @@
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="55">
+  <cellStyles count="79">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -966,6 +1021,18 @@
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -993,6 +1060,18 @@
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1026,7 +1105,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'PON-SVAVA-MATCH'!$M$5</c:f>
+              <c:f>'PON-SVAVA-MATCH'!$O$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1057,7 +1136,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'PON-SVAVA-MATCH'!$N$4:$P$4</c:f>
+              <c:f>'PON-SVAVA-MATCH'!$P$4:$R$4</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1074,7 +1153,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'PON-SVAVA-MATCH'!$N$5:$P$5</c:f>
+              <c:f>'PON-SVAVA-MATCH'!$P$5:$R$5</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1096,7 +1175,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'PON-SVAVA-MATCH'!$M$6</c:f>
+              <c:f>'PON-SVAVA-MATCH'!$O$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1127,7 +1206,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'PON-SVAVA-MATCH'!$N$4:$P$4</c:f>
+              <c:f>'PON-SVAVA-MATCH'!$P$4:$R$4</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1144,7 +1223,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'PON-SVAVA-MATCH'!$N$6:$P$6</c:f>
+              <c:f>'PON-SVAVA-MATCH'!$P$6:$R$6</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1166,7 +1245,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'PON-SVAVA-MATCH'!$M$7</c:f>
+              <c:f>'PON-SVAVA-MATCH'!$O$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1197,7 +1276,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'PON-SVAVA-MATCH'!$N$4:$P$4</c:f>
+              <c:f>'PON-SVAVA-MATCH'!$P$4:$R$4</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1214,7 +1293,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'PON-SVAVA-MATCH'!$N$7:$P$7</c:f>
+              <c:f>'PON-SVAVA-MATCH'!$P$7:$R$7</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1240,11 +1319,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2129793352"/>
-        <c:axId val="2130061064"/>
+        <c:axId val="-2146077000"/>
+        <c:axId val="2137935816"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2129793352"/>
+        <c:axId val="-2146077000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1263,7 +1342,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2130061064"/>
+        <c:crossAx val="2137935816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1271,7 +1350,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2130061064"/>
+        <c:axId val="2137935816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1292,7 +1371,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2129793352"/>
+        <c:crossAx val="-2146077000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1324,24 +1403,431 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.149562685261357"/>
+          <c:y val="0.0388889850307173"/>
+          <c:w val="0.726994946527206"/>
+          <c:h val="0.879274934383202"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'unique  per tool'!$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Delly</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'unique  per tool'!$C$5:$G$5</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>DEL</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>DUP</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>INS</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>INV</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>TRA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'unique  per tool'!$C$6:$G$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1624.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>934.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>389.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>514.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'unique  per tool'!$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Manta</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'unique  per tool'!$C$5:$G$5</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>DEL</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>DUP</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>INS</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>INV</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>TRA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'unique  per tool'!$C$7:$G$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1117.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>475.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>953.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1537.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'unique  per tool'!$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Svaba</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'unique  per tool'!$C$5:$G$5</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>DEL</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>DUP</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>INS</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>INV</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>TRA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'unique  per tool'!$C$8:$G$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4954.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>402.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="-2145540072"/>
+        <c:axId val="-2145534936"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2145540072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2145534936"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2145534936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2145540072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>749300</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2068,7 +2554,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2313,7 +2798,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2932,7 +3416,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2943,10 +3426,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:Q61"/>
+  <dimension ref="C2:S62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="N61" sqref="N61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2959,24 +3442,24 @@
     <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:17">
-      <c r="D2" s="2" t="s">
+    <row r="2" spans="3:19">
+      <c r="D2" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2" t="s">
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2" t="s">
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-    </row>
-    <row r="3" spans="3:17">
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+    </row>
+    <row r="3" spans="3:19">
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
         <v>256</v>
@@ -3005,8 +3488,11 @@
       <c r="L3" s="1" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="4" spans="3:17">
+      <c r="M3" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="4" spans="3:19">
       <c r="C4" s="1" t="s">
         <v>197</v>
       </c>
@@ -3040,20 +3526,27 @@
         <f>J4-K4</f>
         <v>16</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="M4">
+        <v>13</v>
+      </c>
+      <c r="N4">
+        <f>M4/L4</f>
+        <v>0.8125</v>
+      </c>
+      <c r="P4" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="S4" s="1" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="5" spans="3:17">
+    <row r="5" spans="3:19">
       <c r="C5" s="1" t="s">
         <v>198</v>
       </c>
@@ -3087,24 +3580,31 @@
         <f t="shared" ref="L5:L60" si="2">J5-K5</f>
         <v>35</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5">
+        <v>26</v>
+      </c>
+      <c r="N5">
+        <f t="shared" ref="N5:N12" si="3">M5/L5</f>
+        <v>0.74285714285714288</v>
+      </c>
+      <c r="O5" t="s">
         <v>259</v>
       </c>
-      <c r="N5" s="3">
+      <c r="P5" s="3">
         <v>12528</v>
       </c>
-      <c r="O5" s="3">
+      <c r="Q5" s="3">
         <v>1919</v>
       </c>
-      <c r="P5" s="3">
+      <c r="R5" s="3">
         <v>10609</v>
       </c>
-      <c r="Q5" s="3">
-        <f>O5/N5*100</f>
+      <c r="S5" s="3">
+        <f>Q5/P5*100</f>
         <v>15.317688378033207</v>
       </c>
     </row>
-    <row r="6" spans="3:17">
+    <row r="6" spans="3:19">
       <c r="C6" s="1" t="s">
         <v>199</v>
       </c>
@@ -3138,24 +3638,31 @@
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6">
+        <v>17</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="3"/>
+        <v>0.85</v>
+      </c>
+      <c r="O6" t="s">
         <v>260</v>
       </c>
-      <c r="N6" s="3">
+      <c r="P6" s="3">
         <v>10288</v>
       </c>
-      <c r="O6" s="3">
+      <c r="Q6" s="3">
         <v>850</v>
       </c>
-      <c r="P6" s="3">
+      <c r="R6" s="3">
         <v>9438</v>
       </c>
-      <c r="Q6" s="3">
-        <f t="shared" ref="Q6:Q7" si="3">O6/N6*100</f>
+      <c r="S6" s="3">
+        <f>Q6/P6*100</f>
         <v>8.2620528771384141</v>
       </c>
     </row>
-    <row r="7" spans="3:17">
+    <row r="7" spans="3:19">
       <c r="C7" s="1" t="s">
         <v>200</v>
       </c>
@@ -3189,24 +3696,31 @@
         <f t="shared" si="2"/>
         <v>155</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7">
+        <v>138</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="3"/>
+        <v>0.89032258064516134</v>
+      </c>
+      <c r="O7" t="s">
         <v>261</v>
       </c>
-      <c r="N7" s="3">
+      <c r="P7" s="3">
         <v>6451</v>
       </c>
-      <c r="O7" s="3">
+      <c r="Q7" s="3">
         <v>2292</v>
       </c>
-      <c r="P7" s="3">
+      <c r="R7" s="3">
         <v>4159</v>
       </c>
-      <c r="Q7" s="3">
-        <f t="shared" si="3"/>
+      <c r="S7" s="3">
+        <f>Q7/P7*100</f>
         <v>35.529375290652609</v>
       </c>
     </row>
-    <row r="8" spans="3:17">
+    <row r="8" spans="3:19">
       <c r="C8" s="1" t="s">
         <v>201</v>
       </c>
@@ -3240,8 +3754,15 @@
         <f t="shared" si="2"/>
         <v>170</v>
       </c>
-    </row>
-    <row r="9" spans="3:17">
+      <c r="M8">
+        <v>156</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="3"/>
+        <v>0.91764705882352937</v>
+      </c>
+    </row>
+    <row r="9" spans="3:19">
       <c r="C9" s="1" t="s">
         <v>202</v>
       </c>
@@ -3275,8 +3796,15 @@
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="3:17">
+      <c r="M9">
+        <v>14</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="3"/>
+        <v>0.73684210526315785</v>
+      </c>
+    </row>
+    <row r="10" spans="3:19">
       <c r="C10" s="1" t="s">
         <v>203</v>
       </c>
@@ -3310,8 +3838,15 @@
         <f t="shared" si="2"/>
         <v>44</v>
       </c>
-    </row>
-    <row r="11" spans="3:17">
+      <c r="M10">
+        <v>42</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="3"/>
+        <v>0.95454545454545459</v>
+      </c>
+    </row>
+    <row r="11" spans="3:19">
       <c r="C11" s="1" t="s">
         <v>204</v>
       </c>
@@ -3345,8 +3880,15 @@
         <f t="shared" si="2"/>
         <v>169</v>
       </c>
-    </row>
-    <row r="12" spans="3:17">
+      <c r="M11">
+        <v>165</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="3"/>
+        <v>0.97633136094674555</v>
+      </c>
+    </row>
+    <row r="12" spans="3:19">
       <c r="C12" s="1" t="s">
         <v>205</v>
       </c>
@@ -3380,8 +3922,15 @@
         <f t="shared" si="2"/>
         <v>70</v>
       </c>
-    </row>
-    <row r="13" spans="3:17">
+      <c r="M12">
+        <v>65</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="3"/>
+        <v>0.9285714285714286</v>
+      </c>
+    </row>
+    <row r="13" spans="3:19">
       <c r="C13" s="1" t="s">
         <v>206</v>
       </c>
@@ -3415,8 +3964,15 @@
         <f t="shared" si="2"/>
         <v>160</v>
       </c>
-    </row>
-    <row r="14" spans="3:17">
+      <c r="M13">
+        <v>154</v>
+      </c>
+      <c r="N13">
+        <f>M13/L13</f>
+        <v>0.96250000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="3:19">
       <c r="C14" s="1" t="s">
         <v>207</v>
       </c>
@@ -3450,8 +4006,15 @@
         <f t="shared" si="2"/>
         <v>151</v>
       </c>
-    </row>
-    <row r="15" spans="3:17">
+      <c r="M14">
+        <v>144</v>
+      </c>
+      <c r="N14">
+        <f t="shared" ref="N14:N59" si="4">M14/L14</f>
+        <v>0.95364238410596025</v>
+      </c>
+    </row>
+    <row r="15" spans="3:19">
       <c r="C15" s="1" t="s">
         <v>208</v>
       </c>
@@ -3485,8 +4048,15 @@
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-    </row>
-    <row r="16" spans="3:17">
+      <c r="M15">
+        <v>15</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="4"/>
+        <v>0.78947368421052633</v>
+      </c>
+    </row>
+    <row r="16" spans="3:19">
       <c r="C16" s="1" t="s">
         <v>209</v>
       </c>
@@ -3520,8 +4090,15 @@
         <f t="shared" si="2"/>
         <v>99</v>
       </c>
-    </row>
-    <row r="17" spans="3:12">
+      <c r="M16">
+        <v>91</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="4"/>
+        <v>0.91919191919191923</v>
+      </c>
+    </row>
+    <row r="17" spans="3:14">
       <c r="C17" s="1" t="s">
         <v>210</v>
       </c>
@@ -3555,8 +4132,15 @@
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="3:12">
+      <c r="M17">
+        <v>20</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="3:14">
       <c r="C18" s="1" t="s">
         <v>211</v>
       </c>
@@ -3590,8 +4174,15 @@
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-    </row>
-    <row r="19" spans="3:12">
+      <c r="M18">
+        <v>23</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="4"/>
+        <v>0.95833333333333337</v>
+      </c>
+    </row>
+    <row r="19" spans="3:14">
       <c r="C19" s="1" t="s">
         <v>212</v>
       </c>
@@ -3625,8 +4216,15 @@
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="3:12">
+      <c r="M19">
+        <v>16</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="4"/>
+        <v>0.88888888888888884</v>
+      </c>
+    </row>
+    <row r="20" spans="3:14">
       <c r="C20" s="1" t="s">
         <v>213</v>
       </c>
@@ -3660,8 +4258,15 @@
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-    </row>
-    <row r="21" spans="3:12">
+      <c r="M20">
+        <v>19</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="4"/>
+        <v>0.86363636363636365</v>
+      </c>
+    </row>
+    <row r="21" spans="3:14">
       <c r="C21" s="1" t="s">
         <v>214</v>
       </c>
@@ -3695,8 +4300,15 @@
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="22" spans="3:12">
+      <c r="M21">
+        <v>11</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="4"/>
+        <v>0.73333333333333328</v>
+      </c>
+    </row>
+    <row r="22" spans="3:14">
       <c r="C22" s="1" t="s">
         <v>215</v>
       </c>
@@ -3730,8 +4342,15 @@
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="23" spans="3:12">
+      <c r="M22">
+        <v>16</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="4"/>
+        <v>0.88888888888888884</v>
+      </c>
+    </row>
+    <row r="23" spans="3:14">
       <c r="C23" s="1" t="s">
         <v>216</v>
       </c>
@@ -3765,8 +4384,15 @@
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="24" spans="3:12">
+      <c r="M23">
+        <v>14</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="4"/>
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="24" spans="3:14">
       <c r="C24" s="1" t="s">
         <v>217</v>
       </c>
@@ -3800,8 +4426,15 @@
         <f t="shared" si="2"/>
         <v>159</v>
       </c>
-    </row>
-    <row r="25" spans="3:12">
+      <c r="M24">
+        <v>151</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="4"/>
+        <v>0.94968553459119498</v>
+      </c>
+    </row>
+    <row r="25" spans="3:14">
       <c r="C25" s="1" t="s">
         <v>218</v>
       </c>
@@ -3835,8 +4468,15 @@
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="26" spans="3:12">
+      <c r="M25">
+        <v>12</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="4"/>
+        <v>0.92307692307692313</v>
+      </c>
+    </row>
+    <row r="26" spans="3:14">
       <c r="C26" s="1" t="s">
         <v>219</v>
       </c>
@@ -3870,8 +4510,15 @@
         <f t="shared" si="2"/>
         <v>91</v>
       </c>
-    </row>
-    <row r="27" spans="3:12">
+      <c r="M26">
+        <v>84</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="4"/>
+        <v>0.92307692307692313</v>
+      </c>
+    </row>
+    <row r="27" spans="3:14">
       <c r="C27" s="1" t="s">
         <v>220</v>
       </c>
@@ -3905,8 +4552,15 @@
         <f t="shared" si="2"/>
         <v>69</v>
       </c>
-    </row>
-    <row r="28" spans="3:12">
+      <c r="M27">
+        <v>61</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="4"/>
+        <v>0.88405797101449279</v>
+      </c>
+    </row>
+    <row r="28" spans="3:14">
       <c r="C28" s="1" t="s">
         <v>221</v>
       </c>
@@ -3940,8 +4594,15 @@
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
-    </row>
-    <row r="29" spans="3:12">
+      <c r="M28">
+        <v>30</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="4"/>
+        <v>0.88235294117647056</v>
+      </c>
+    </row>
+    <row r="29" spans="3:14">
       <c r="C29" s="1" t="s">
         <v>222</v>
       </c>
@@ -3975,8 +4636,15 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="3:12">
+      <c r="M29">
+        <v>4</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="3:14">
       <c r="C30" s="1" t="s">
         <v>223</v>
       </c>
@@ -4010,8 +4678,15 @@
         <f t="shared" si="2"/>
         <v>80</v>
       </c>
-    </row>
-    <row r="31" spans="3:12">
+      <c r="M30">
+        <v>79</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="4"/>
+        <v>0.98750000000000004</v>
+      </c>
+    </row>
+    <row r="31" spans="3:14">
       <c r="C31" s="1" t="s">
         <v>224</v>
       </c>
@@ -4045,8 +4720,15 @@
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="32" spans="3:12">
+      <c r="M31">
+        <v>11</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="4"/>
+        <v>0.7857142857142857</v>
+      </c>
+    </row>
+    <row r="32" spans="3:14">
       <c r="C32" s="1" t="s">
         <v>225</v>
       </c>
@@ -4080,8 +4762,15 @@
         <f t="shared" si="2"/>
         <v>292</v>
       </c>
-    </row>
-    <row r="33" spans="3:12">
+      <c r="M32">
+        <v>285</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="4"/>
+        <v>0.97602739726027399</v>
+      </c>
+    </row>
+    <row r="33" spans="3:14">
       <c r="C33" s="1" t="s">
         <v>226</v>
       </c>
@@ -4115,8 +4804,15 @@
         <f t="shared" si="2"/>
         <v>353</v>
       </c>
-    </row>
-    <row r="34" spans="3:12">
+      <c r="M33">
+        <v>349</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="4"/>
+        <v>0.98866855524079322</v>
+      </c>
+    </row>
+    <row r="34" spans="3:14">
       <c r="C34" s="1" t="s">
         <v>227</v>
       </c>
@@ -4150,8 +4846,15 @@
         <f t="shared" si="2"/>
         <v>115</v>
       </c>
-    </row>
-    <row r="35" spans="3:12">
+      <c r="M34">
+        <v>110</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="4"/>
+        <v>0.95652173913043481</v>
+      </c>
+    </row>
+    <row r="35" spans="3:14">
       <c r="C35" s="1" t="s">
         <v>228</v>
       </c>
@@ -4185,8 +4888,15 @@
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="36" spans="3:12">
+      <c r="M35">
+        <v>26</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="4"/>
+        <v>0.72222222222222221</v>
+      </c>
+    </row>
+    <row r="36" spans="3:14">
       <c r="C36" s="1" t="s">
         <v>229</v>
       </c>
@@ -4220,8 +4930,15 @@
         <f t="shared" si="2"/>
         <v>132</v>
       </c>
-    </row>
-    <row r="37" spans="3:12">
+      <c r="M36">
+        <v>124</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="4"/>
+        <v>0.93939393939393945</v>
+      </c>
+    </row>
+    <row r="37" spans="3:14">
       <c r="C37" s="1" t="s">
         <v>230</v>
       </c>
@@ -4255,8 +4972,15 @@
         <f t="shared" si="2"/>
         <v>152</v>
       </c>
-    </row>
-    <row r="38" spans="3:12">
+      <c r="M37">
+        <v>138</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="4"/>
+        <v>0.90789473684210531</v>
+      </c>
+    </row>
+    <row r="38" spans="3:14">
       <c r="C38" s="1" t="s">
         <v>231</v>
       </c>
@@ -4290,8 +5014,15 @@
         <f t="shared" si="2"/>
         <v>155</v>
       </c>
-    </row>
-    <row r="39" spans="3:12">
+      <c r="M38">
+        <v>139</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="4"/>
+        <v>0.89677419354838706</v>
+      </c>
+    </row>
+    <row r="39" spans="3:14">
       <c r="C39" s="1" t="s">
         <v>232</v>
       </c>
@@ -4325,8 +5056,15 @@
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="40" spans="3:12">
+      <c r="M39">
+        <v>8</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="4"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="40" spans="3:14">
       <c r="C40" s="1" t="s">
         <v>233</v>
       </c>
@@ -4360,8 +5098,15 @@
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="41" spans="3:12">
+      <c r="M40">
+        <v>13</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="4"/>
+        <v>0.9285714285714286</v>
+      </c>
+    </row>
+    <row r="41" spans="3:14">
       <c r="C41" s="1" t="s">
         <v>234</v>
       </c>
@@ -4395,8 +5140,15 @@
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="42" spans="3:12">
+      <c r="M41">
+        <v>14</v>
+      </c>
+      <c r="N41">
+        <f t="shared" si="4"/>
+        <v>0.77777777777777779</v>
+      </c>
+    </row>
+    <row r="42" spans="3:14">
       <c r="C42" s="1" t="s">
         <v>235</v>
       </c>
@@ -4430,8 +5182,15 @@
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-    </row>
-    <row r="43" spans="3:12">
+      <c r="M42">
+        <v>22</v>
+      </c>
+      <c r="N42">
+        <f t="shared" si="4"/>
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="43" spans="3:14">
       <c r="C43" s="1" t="s">
         <v>236</v>
       </c>
@@ -4465,8 +5224,15 @@
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-    </row>
-    <row r="44" spans="3:12">
+      <c r="M43">
+        <v>43</v>
+      </c>
+      <c r="N43">
+        <f t="shared" si="4"/>
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="44" spans="3:14">
       <c r="C44" s="1" t="s">
         <v>237</v>
       </c>
@@ -4500,8 +5266,15 @@
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="45" spans="3:12">
+      <c r="M44">
+        <v>16</v>
+      </c>
+      <c r="N44">
+        <f t="shared" si="4"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="45" spans="3:14">
       <c r="C45" s="1" t="s">
         <v>238</v>
       </c>
@@ -4535,8 +5308,15 @@
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-    </row>
-    <row r="46" spans="3:12">
+      <c r="M45">
+        <v>18</v>
+      </c>
+      <c r="N45">
+        <f t="shared" si="4"/>
+        <v>0.81818181818181823</v>
+      </c>
+    </row>
+    <row r="46" spans="3:14">
       <c r="C46" s="1" t="s">
         <v>239</v>
       </c>
@@ -4570,8 +5350,15 @@
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
-    </row>
-    <row r="47" spans="3:12">
+      <c r="M46">
+        <v>22</v>
+      </c>
+      <c r="N46">
+        <f t="shared" si="4"/>
+        <v>0.81481481481481477</v>
+      </c>
+    </row>
+    <row r="47" spans="3:14">
       <c r="C47" s="1" t="s">
         <v>240</v>
       </c>
@@ -4605,8 +5392,15 @@
         <f t="shared" si="2"/>
         <v>56</v>
       </c>
-    </row>
-    <row r="48" spans="3:12">
+      <c r="M47">
+        <v>51</v>
+      </c>
+      <c r="N47">
+        <f t="shared" si="4"/>
+        <v>0.9107142857142857</v>
+      </c>
+    </row>
+    <row r="48" spans="3:14">
       <c r="C48" s="1" t="s">
         <v>241</v>
       </c>
@@ -4640,8 +5434,15 @@
         <f t="shared" si="2"/>
         <v>306</v>
       </c>
-    </row>
-    <row r="49" spans="3:12">
+      <c r="M48">
+        <v>298</v>
+      </c>
+      <c r="N48">
+        <f t="shared" si="4"/>
+        <v>0.97385620915032678</v>
+      </c>
+    </row>
+    <row r="49" spans="3:14">
       <c r="C49" s="1" t="s">
         <v>242</v>
       </c>
@@ -4675,8 +5476,15 @@
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
-    </row>
-    <row r="50" spans="3:12">
+      <c r="M49">
+        <v>30</v>
+      </c>
+      <c r="N49">
+        <f t="shared" si="4"/>
+        <v>0.78947368421052633</v>
+      </c>
+    </row>
+    <row r="50" spans="3:14">
       <c r="C50" s="1" t="s">
         <v>243</v>
       </c>
@@ -4710,8 +5518,15 @@
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-    </row>
-    <row r="51" spans="3:12">
+      <c r="M50">
+        <v>23</v>
+      </c>
+      <c r="N50">
+        <f t="shared" si="4"/>
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="51" spans="3:14">
       <c r="C51" s="1" t="s">
         <v>244</v>
       </c>
@@ -4745,8 +5560,15 @@
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="52" spans="3:12">
+      <c r="M51">
+        <v>13</v>
+      </c>
+      <c r="N51">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="3:14">
       <c r="C52" s="1" t="s">
         <v>245</v>
       </c>
@@ -4780,8 +5602,15 @@
         <f t="shared" si="2"/>
         <v>107</v>
       </c>
-    </row>
-    <row r="53" spans="3:12">
+      <c r="M52">
+        <v>103</v>
+      </c>
+      <c r="N52">
+        <f t="shared" si="4"/>
+        <v>0.96261682242990654</v>
+      </c>
+    </row>
+    <row r="53" spans="3:14">
       <c r="C53" s="1" t="s">
         <v>246</v>
       </c>
@@ -4815,8 +5644,15 @@
         <f t="shared" si="2"/>
         <v>58</v>
       </c>
-    </row>
-    <row r="54" spans="3:12">
+      <c r="M53">
+        <v>53</v>
+      </c>
+      <c r="N53">
+        <f t="shared" si="4"/>
+        <v>0.91379310344827591</v>
+      </c>
+    </row>
+    <row r="54" spans="3:14">
       <c r="C54" s="1" t="s">
         <v>247</v>
       </c>
@@ -4850,8 +5686,15 @@
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-    </row>
-    <row r="55" spans="3:12">
+      <c r="M54">
+        <v>15</v>
+      </c>
+      <c r="N54">
+        <f t="shared" si="4"/>
+        <v>0.68181818181818177</v>
+      </c>
+    </row>
+    <row r="55" spans="3:14">
       <c r="C55" s="1" t="s">
         <v>248</v>
       </c>
@@ -4885,8 +5728,15 @@
         <f t="shared" si="2"/>
         <v>141</v>
       </c>
-    </row>
-    <row r="56" spans="3:12">
+      <c r="M55">
+        <v>131</v>
+      </c>
+      <c r="N55">
+        <f t="shared" si="4"/>
+        <v>0.92907801418439717</v>
+      </c>
+    </row>
+    <row r="56" spans="3:14">
       <c r="C56" s="1" t="s">
         <v>249</v>
       </c>
@@ -4920,8 +5770,15 @@
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-    </row>
-    <row r="57" spans="3:12">
+      <c r="M56">
+        <v>19</v>
+      </c>
+      <c r="N56">
+        <f t="shared" si="4"/>
+        <v>0.86363636363636365</v>
+      </c>
+    </row>
+    <row r="57" spans="3:14">
       <c r="C57" s="1" t="s">
         <v>250</v>
       </c>
@@ -4955,8 +5812,15 @@
         <f t="shared" si="2"/>
         <v>159</v>
       </c>
-    </row>
-    <row r="58" spans="3:12">
+      <c r="M57">
+        <v>136</v>
+      </c>
+      <c r="N57">
+        <f t="shared" si="4"/>
+        <v>0.85534591194968557</v>
+      </c>
+    </row>
+    <row r="58" spans="3:14">
       <c r="C58" s="1" t="s">
         <v>251</v>
       </c>
@@ -4990,8 +5854,15 @@
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="59" spans="3:12">
+      <c r="M58">
+        <v>17</v>
+      </c>
+      <c r="N58">
+        <f t="shared" si="4"/>
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="59" spans="3:14">
       <c r="C59" s="1" t="s">
         <v>252</v>
       </c>
@@ -5025,8 +5896,15 @@
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="60" spans="3:12">
+      <c r="M59">
+        <v>13</v>
+      </c>
+      <c r="N59">
+        <f t="shared" si="4"/>
+        <v>0.9285714285714286</v>
+      </c>
+    </row>
+    <row r="60" spans="3:14">
       <c r="C60" s="1" t="s">
         <v>253</v>
       </c>
@@ -5061,7 +5939,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="61" spans="3:12">
+    <row r="61" spans="3:14">
       <c r="C61" s="1"/>
       <c r="D61" s="3">
         <f>SUM(D4:D60)</f>
@@ -5076,28 +5954,74 @@
         <v>10609</v>
       </c>
       <c r="G61" s="3">
-        <f t="shared" ref="G61:I61" si="4">SUM(G4:G60)</f>
+        <f t="shared" ref="G61:I61" si="5">SUM(G4:G60)</f>
         <v>10288</v>
       </c>
       <c r="H61" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>850</v>
       </c>
       <c r="I61" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9438</v>
       </c>
       <c r="J61" s="3">
-        <f t="shared" ref="J61" si="5">SUM(J4:J60)</f>
+        <f t="shared" ref="J61" si="6">SUM(J4:J60)</f>
         <v>6451</v>
       </c>
       <c r="K61" s="3">
-        <f t="shared" ref="K61" si="6">SUM(K4:K60)</f>
+        <f t="shared" ref="K61" si="7">SUM(K4:K60)</f>
         <v>2292</v>
       </c>
       <c r="L61" s="3">
-        <f t="shared" ref="L61" si="7">SUM(L4:L60)</f>
+        <f t="shared" ref="L61" si="8">SUM(L4:L60)</f>
         <v>4159</v>
+      </c>
+      <c r="M61" s="3">
+        <f>SUM(M4:M59)</f>
+        <v>3820</v>
+      </c>
+      <c r="N61" s="6">
+        <f>M61/L61</f>
+        <v>0.9184900216398173</v>
+      </c>
+    </row>
+    <row r="62" spans="3:14">
+      <c r="D62" s="3">
+        <f>MEDIAN(D4:D60)</f>
+        <v>172</v>
+      </c>
+      <c r="E62" s="3">
+        <f t="shared" ref="E62:L62" si="9">MEDIAN(E4:E60)</f>
+        <v>30</v>
+      </c>
+      <c r="F62" s="3">
+        <f t="shared" si="9"/>
+        <v>138</v>
+      </c>
+      <c r="G62" s="3">
+        <f t="shared" si="9"/>
+        <v>146</v>
+      </c>
+      <c r="H62" s="3">
+        <f t="shared" si="9"/>
+        <v>14</v>
+      </c>
+      <c r="I62" s="3">
+        <f t="shared" si="9"/>
+        <v>127</v>
+      </c>
+      <c r="J62" s="3">
+        <f t="shared" si="9"/>
+        <v>76</v>
+      </c>
+      <c r="K62" s="3">
+        <f t="shared" si="9"/>
+        <v>39</v>
+      </c>
+      <c r="L62" s="3">
+        <f t="shared" si="9"/>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -5115,4 +6039,103 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B5:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="5" spans="2:7">
+      <c r="C5" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="B6" t="s">
+        <v>268</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1624</v>
+      </c>
+      <c r="D6" s="2">
+        <v>934</v>
+      </c>
+      <c r="E6" s="2">
+        <v>2</v>
+      </c>
+      <c r="F6" s="2">
+        <v>389</v>
+      </c>
+      <c r="G6" s="2">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="B7" t="s">
+        <v>260</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1117</v>
+      </c>
+      <c r="D7" s="2">
+        <v>475</v>
+      </c>
+      <c r="E7" s="2">
+        <v>16</v>
+      </c>
+      <c r="F7" s="2">
+        <v>953</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1537</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" t="s">
+        <v>259</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <v>4954</v>
+      </c>
+      <c r="G8" s="2">
+        <v>402</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adding the Rcode per caller to train and predict somatic SVs
</commit_message>
<xml_diff>
--- a/misc/SV-features.xlsx
+++ b/misc/SV-features.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="7940" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="DELLY" sheetId="1" r:id="rId1"/>
     <sheet name="MANTA" sheetId="2" r:id="rId2"/>
     <sheet name="SVABA" sheetId="3" r:id="rId3"/>
-    <sheet name="PON-SVAVA-MATCH" sheetId="4" r:id="rId4"/>
-    <sheet name="unique  per tool" sheetId="5" r:id="rId5"/>
+    <sheet name="RF-model-v1" sheetId="6" r:id="rId4"/>
+    <sheet name="PON-SVAVA-MATCH" sheetId="4" r:id="rId5"/>
+    <sheet name="unique  per tool" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="303">
   <si>
     <t>CIEND</t>
   </si>
@@ -833,16 +834,117 @@
   </si>
   <si>
     <t>PONF</t>
+  </si>
+  <si>
+    <t>PON_BC1</t>
+  </si>
+  <si>
+    <t>PON_BC2</t>
+  </si>
+  <si>
+    <t>GNOMAD_AC</t>
+  </si>
+  <si>
+    <t>GNOMAD_BC1</t>
+  </si>
+  <si>
+    <t>GNOMAD_BC2</t>
+  </si>
+  <si>
+    <t>PCAWG_BC1</t>
+  </si>
+  <si>
+    <t>PCAWG_BC2</t>
+  </si>
+  <si>
+    <t>COSMIC_GENE</t>
+  </si>
+  <si>
+    <t>CENTROMER</t>
+  </si>
+  <si>
+    <t>EXON</t>
+  </si>
+  <si>
+    <t>CONSERVATION_BC1</t>
+  </si>
+  <si>
+    <t>CONSERVATION_BC2</t>
+  </si>
+  <si>
+    <t>CNV_TCN1</t>
+  </si>
+  <si>
+    <t>CNV_TCN2</t>
+  </si>
+  <si>
+    <t>CNV_CF1</t>
+  </si>
+  <si>
+    <t>CNV_CF2</t>
+  </si>
+  <si>
+    <t>RAF</t>
+  </si>
+  <si>
+    <t>RFS</t>
+  </si>
+  <si>
+    <t>DELLY</t>
+  </si>
+  <si>
+    <t>TP</t>
+  </si>
+  <si>
+    <t>FP</t>
+  </si>
+  <si>
+    <t>GERMLINE</t>
+  </si>
+  <si>
+    <t>FN</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>ACC</t>
+  </si>
+  <si>
+    <t>FDR</t>
+  </si>
+  <si>
+    <t>FNR</t>
+  </si>
+  <si>
+    <t>Precision</t>
+  </si>
+  <si>
+    <t>recall</t>
+  </si>
+  <si>
+    <t>Caller</t>
+  </si>
+  <si>
+    <t>Recall</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -873,6 +975,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -891,7 +1001,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="79">
+  <cellStyleXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -971,8 +1081,54 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -992,8 +1148,26 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="79">
+  <cellStyles count="125">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1033,6 +1207,29 @@
     <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1072,6 +1269,29 @@
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1319,11 +1539,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2146077000"/>
-        <c:axId val="2137935816"/>
+        <c:axId val="-2139714232"/>
+        <c:axId val="-2141425368"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2146077000"/>
+        <c:axId val="-2139714232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1342,7 +1562,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2137935816"/>
+        <c:crossAx val="-2141425368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1350,7 +1570,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2137935816"/>
+        <c:axId val="-2141425368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1371,7 +1591,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2146077000"/>
+        <c:crossAx val="-2139714232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1682,11 +1902,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2145540072"/>
-        <c:axId val="-2145534936"/>
+        <c:axId val="-2141250664"/>
+        <c:axId val="-2141247528"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2145540072"/>
+        <c:axId val="-2141250664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1705,7 +1925,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2145534936"/>
+        <c:crossAx val="-2141247528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1713,7 +1933,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2145534936"/>
+        <c:axId val="-2141247528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1733,7 +1953,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2145540072"/>
+        <c:crossAx val="-2141250664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2169,8 +2389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C15"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2811,7 +3031,7 @@
   <dimension ref="B1:D54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B2:H31"/>
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3426,10 +3646,703 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:U33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:21">
+      <c r="C4" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="D4" t="s">
+        <v>258</v>
+      </c>
+      <c r="E4" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="5" spans="2:21">
+      <c r="B5" t="s">
+        <v>270</v>
+      </c>
+      <c r="C5" s="11">
+        <v>449.60410999999999</v>
+      </c>
+      <c r="D5" s="11">
+        <v>1145.7990600000001</v>
+      </c>
+      <c r="E5" s="11">
+        <v>1051.174495</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21">
+      <c r="B6" t="s">
+        <v>271</v>
+      </c>
+      <c r="C6" s="11">
+        <v>529.30900999999994</v>
+      </c>
+      <c r="D6" s="11">
+        <v>1239.5422100000001</v>
+      </c>
+      <c r="E6" s="11">
+        <v>908.03942199999995</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="O6" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="P6" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="Q6" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="R6" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="S6" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="T6" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="U6" s="8" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21">
+      <c r="B7" t="s">
+        <v>272</v>
+      </c>
+      <c r="C7" s="11">
+        <v>122.85713</v>
+      </c>
+      <c r="D7" s="11">
+        <v>218.8373</v>
+      </c>
+      <c r="E7" s="11">
+        <v>271.82045900000003</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="K7" s="5">
+        <v>1</v>
+      </c>
+      <c r="L7" s="5">
+        <v>1384</v>
+      </c>
+      <c r="M7" s="5">
+        <v>136</v>
+      </c>
+      <c r="N7" s="5">
+        <v>0</v>
+      </c>
+      <c r="O7" s="5">
+        <v>173</v>
+      </c>
+      <c r="P7" s="5">
+        <v>1421</v>
+      </c>
+      <c r="Q7" s="9">
+        <f t="shared" ref="Q7:Q9" si="0">SUM(L7+P7)/SUM(L7+M7+O7+P7)</f>
+        <v>0.90077071290944122</v>
+      </c>
+      <c r="R7" s="9">
+        <f t="shared" ref="R7:R9" si="1">M7/(L7+M7)</f>
+        <v>8.9473684210526316E-2</v>
+      </c>
+      <c r="S7" s="5">
+        <f>O7/SUM(L7+O7)</f>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="T7" s="9">
+        <f>1-R7</f>
+        <v>0.91052631578947363</v>
+      </c>
+      <c r="U7" s="5">
+        <f>1-S7</f>
+        <v>0.88888888888888884</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21">
+      <c r="B8" t="s">
+        <v>273</v>
+      </c>
+      <c r="C8" s="11">
+        <v>108.72526999999999</v>
+      </c>
+      <c r="D8" s="11">
+        <v>146.44056</v>
+      </c>
+      <c r="E8" s="11">
+        <v>105.447174</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="K8" s="5">
+        <v>1</v>
+      </c>
+      <c r="L8" s="5">
+        <v>1803</v>
+      </c>
+      <c r="M8" s="5">
+        <v>213</v>
+      </c>
+      <c r="N8" s="5">
+        <v>0</v>
+      </c>
+      <c r="O8" s="5">
+        <v>287</v>
+      </c>
+      <c r="P8" s="5">
+        <v>1877</v>
+      </c>
+      <c r="Q8" s="9">
+        <f t="shared" si="0"/>
+        <v>0.88038277511961727</v>
+      </c>
+      <c r="R8" s="9">
+        <f t="shared" si="1"/>
+        <v>0.1056547619047619</v>
+      </c>
+      <c r="S8" s="5">
+        <f>O8/SUM(L8+O8)</f>
+        <v>0.13732057416267943</v>
+      </c>
+      <c r="T8" s="9">
+        <f>1-R8</f>
+        <v>0.89434523809523814</v>
+      </c>
+      <c r="U8" s="5">
+        <f>1-S8</f>
+        <v>0.8626794258373206</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21">
+      <c r="B9" t="s">
+        <v>274</v>
+      </c>
+      <c r="C9" s="11">
+        <v>112.92413000000001</v>
+      </c>
+      <c r="D9" s="11">
+        <v>144.52603999999999</v>
+      </c>
+      <c r="E9" s="11">
+        <v>99.268625999999998</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="K9" s="5">
+        <v>1</v>
+      </c>
+      <c r="L9" s="5">
+        <v>1317</v>
+      </c>
+      <c r="M9" s="5">
+        <v>131</v>
+      </c>
+      <c r="N9" s="5">
+        <v>0</v>
+      </c>
+      <c r="O9" s="5">
+        <v>216</v>
+      </c>
+      <c r="P9" s="5">
+        <v>1402</v>
+      </c>
+      <c r="Q9" s="9">
+        <f t="shared" si="0"/>
+        <v>0.88682322243966083</v>
+      </c>
+      <c r="R9" s="9">
+        <f t="shared" si="1"/>
+        <v>9.0469613259668513E-2</v>
+      </c>
+      <c r="S9" s="5">
+        <f>O9/SUM(L9+O9)</f>
+        <v>0.14090019569471623</v>
+      </c>
+      <c r="T9" s="9">
+        <f>1-R9</f>
+        <v>0.90953038674033149</v>
+      </c>
+      <c r="U9" s="5">
+        <f>1-S9</f>
+        <v>0.85909980430528377</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21">
+      <c r="B10" t="s">
+        <v>275</v>
+      </c>
+      <c r="C10" s="11">
+        <v>95.127480000000006</v>
+      </c>
+      <c r="D10" s="11">
+        <v>133.23260999999999</v>
+      </c>
+      <c r="E10" s="11">
+        <v>86.687217000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21">
+      <c r="B11" t="s">
+        <v>276</v>
+      </c>
+      <c r="C11" s="11">
+        <v>93.777699999999996</v>
+      </c>
+      <c r="D11" s="11">
+        <v>130.42103</v>
+      </c>
+      <c r="E11" s="11">
+        <v>87.642632000000006</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21">
+      <c r="B12" t="s">
+        <v>277</v>
+      </c>
+      <c r="C12" s="11">
+        <v>10.528090000000001</v>
+      </c>
+      <c r="D12" s="11">
+        <v>12.568479999999999</v>
+      </c>
+      <c r="E12" s="11">
+        <v>8.6654180000000007</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21">
+      <c r="B13" t="s">
+        <v>278</v>
+      </c>
+      <c r="C13" s="11">
+        <v>12.98352</v>
+      </c>
+      <c r="D13" s="11">
+        <v>27.458089999999999</v>
+      </c>
+      <c r="E13" s="11">
+        <v>25.684902000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21">
+      <c r="B14" t="s">
+        <v>279</v>
+      </c>
+      <c r="C14" s="11">
+        <v>12.28036</v>
+      </c>
+      <c r="D14" s="11">
+        <v>17.778770000000002</v>
+      </c>
+      <c r="E14" s="11">
+        <v>13.563642</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="M14" s="5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21">
+      <c r="B15" t="s">
+        <v>280</v>
+      </c>
+      <c r="C15" s="11">
+        <v>135.68983</v>
+      </c>
+      <c r="D15" s="11">
+        <v>195.79732000000001</v>
+      </c>
+      <c r="E15" s="11">
+        <v>128.14271400000001</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="K15" s="3">
+        <v>1</v>
+      </c>
+      <c r="L15" s="3">
+        <v>1</v>
+      </c>
+      <c r="M15" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:21">
+      <c r="B16" t="s">
+        <v>281</v>
+      </c>
+      <c r="C16" s="11">
+        <v>131.32606000000001</v>
+      </c>
+      <c r="D16" s="11">
+        <v>193.13987</v>
+      </c>
+      <c r="E16" s="11">
+        <v>130.91719599999999</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="K16" s="3">
+        <v>1384</v>
+      </c>
+      <c r="L16" s="3">
+        <v>1803</v>
+      </c>
+      <c r="M16" s="3">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13">
+      <c r="B17" t="s">
+        <v>282</v>
+      </c>
+      <c r="C17" s="11">
+        <v>47.9908</v>
+      </c>
+      <c r="D17" s="11">
+        <v>57.562339999999999</v>
+      </c>
+      <c r="E17" s="11">
+        <v>40.737358999999998</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="K17" s="3">
+        <v>136</v>
+      </c>
+      <c r="L17" s="3">
+        <v>213</v>
+      </c>
+      <c r="M17" s="3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13">
+      <c r="B18" t="s">
+        <v>283</v>
+      </c>
+      <c r="C18" s="11">
+        <v>43.397759999999998</v>
+      </c>
+      <c r="D18" s="11">
+        <v>56.118679999999998</v>
+      </c>
+      <c r="E18" s="11">
+        <v>40.408118999999999</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="K18" s="3">
+        <v>0</v>
+      </c>
+      <c r="L18" s="3">
+        <v>0</v>
+      </c>
+      <c r="M18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13">
+      <c r="B19" t="s">
+        <v>284</v>
+      </c>
+      <c r="C19" s="11">
+        <v>106.4315</v>
+      </c>
+      <c r="D19" s="11">
+        <v>128.84486000000001</v>
+      </c>
+      <c r="E19" s="11">
+        <v>79.596627999999995</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="K19" s="3">
+        <v>173</v>
+      </c>
+      <c r="L19" s="3">
+        <v>287</v>
+      </c>
+      <c r="M19" s="3">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13">
+      <c r="B20" t="s">
+        <v>285</v>
+      </c>
+      <c r="C20" s="11">
+        <v>132.23036999999999</v>
+      </c>
+      <c r="D20" s="11">
+        <v>126.90754</v>
+      </c>
+      <c r="E20" s="11">
+        <v>88.671910999999994</v>
+      </c>
+      <c r="J20" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="K20" s="3">
+        <v>1421</v>
+      </c>
+      <c r="L20" s="3">
+        <v>1877</v>
+      </c>
+      <c r="M20" s="3">
+        <v>1402</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13">
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="11">
+        <v>333.15436</v>
+      </c>
+      <c r="D21" s="11">
+        <v>382.29725999999999</v>
+      </c>
+      <c r="E21" s="11">
+        <v>419.42135200000001</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="K21" s="10">
+        <f>SUM(K16+K20)/SUM(K16+K17+K19+K20)</f>
+        <v>0.90077071290944122</v>
+      </c>
+      <c r="L21" s="10">
+        <f>SUM(L16+L20)/SUM(L16+L17+L19+L20)</f>
+        <v>0.88038277511961727</v>
+      </c>
+      <c r="M21" s="10">
+        <f>SUM(M16+M20)/SUM(M16+M17+M19+M20)</f>
+        <v>0.88682322243966083</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13">
+      <c r="B22" t="s">
+        <v>286</v>
+      </c>
+      <c r="C22" s="11">
+        <v>1089.3242600000001</v>
+      </c>
+      <c r="D22" s="11">
+        <v>1106.1222499999999</v>
+      </c>
+      <c r="E22" s="11">
+        <v>465.81873400000001</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="K22" s="10">
+        <f>K17/(K16+K17)</f>
+        <v>8.9473684210526316E-2</v>
+      </c>
+      <c r="L22" s="10">
+        <f>L17/(L16+L17)</f>
+        <v>0.1056547619047619</v>
+      </c>
+      <c r="M22" s="10">
+        <f>M17/(M16+M17)</f>
+        <v>9.0469613259668513E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13">
+      <c r="B23" t="s">
+        <v>287</v>
+      </c>
+      <c r="C23" s="11">
+        <v>1058.8878500000001</v>
+      </c>
+      <c r="D23" s="11">
+        <v>748.19614999999999</v>
+      </c>
+      <c r="E23" s="11">
+        <v>411.89983699999999</v>
+      </c>
+      <c r="J23" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="K23" s="10">
+        <f>K19/SUM(K16+K19)</f>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="L23" s="10">
+        <f>L19/SUM(L16+L19)</f>
+        <v>0.13732057416267943</v>
+      </c>
+      <c r="M23" s="10">
+        <f>M19/SUM(M16+M19)</f>
+        <v>0.14090019569471623</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13">
+      <c r="J24" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="K24" s="10">
+        <f>1-K22</f>
+        <v>0.91052631578947363</v>
+      </c>
+      <c r="L24" s="10">
+        <f>1-L22</f>
+        <v>0.89434523809523814</v>
+      </c>
+      <c r="M24" s="10">
+        <f>1-M22</f>
+        <v>0.90953038674033149</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13">
+      <c r="J25" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="K25" s="10">
+        <f>1-K23</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="L25" s="10">
+        <f>1-L23</f>
+        <v>0.8626794258373206</v>
+      </c>
+      <c r="M25" s="10">
+        <f>1-M23</f>
+        <v>0.85909980430528377</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13">
+      <c r="J29" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="K29" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="L29" s="5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13">
+      <c r="J30">
+        <v>510865</v>
+      </c>
+      <c r="K30">
+        <v>644814</v>
+      </c>
+      <c r="L30">
+        <v>260055</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13">
+      <c r="I31" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="J31" s="3">
+        <f>SUM(J30+J32)</f>
+        <v>519751</v>
+      </c>
+      <c r="K31" s="3">
+        <f>SUM(K30+K32)</f>
+        <v>654029</v>
+      </c>
+      <c r="L31" s="3">
+        <f>SUM(L30+L32)</f>
+        <v>276671</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13">
+      <c r="I32" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="J32" s="3">
+        <v>8886</v>
+      </c>
+      <c r="K32" s="3">
+        <v>9215</v>
+      </c>
+      <c r="L32" s="3">
+        <v>16616</v>
+      </c>
+    </row>
+    <row r="33" spans="9:12">
+      <c r="I33" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="J33" s="12">
+        <f>J32/J31*100</f>
+        <v>1.709664820269706</v>
+      </c>
+      <c r="K33" s="12">
+        <f t="shared" ref="K33:L33" si="2">K32/K31*100</f>
+        <v>1.4089589299557055</v>
+      </c>
+      <c r="L33" s="12">
+        <f t="shared" si="2"/>
+        <v>6.0056890675206294</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:S62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="N61" sqref="N61"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3443,21 +4356,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:19">
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5" t="s">
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7" t="s">
         <v>258</v>
       </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5" t="s">
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
     </row>
     <row r="3" spans="3:19">
       <c r="C3" s="1"/>
@@ -6031,7 +6944,6 @@
     <mergeCell ref="J2:L2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -6041,12 +6953,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6130,7 +7042,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>